<commit_message>
added link for explanation glm naivebayes
</commit_message>
<xml_diff>
--- a/summaryVotePredictionModels.xlsx
+++ b/summaryVotePredictionModels.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>Sensitivity Rate of True Positives</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>cost=0.5, weight=3</t>
+  </si>
+  <si>
+    <t>https://www.quora.com/What-is-the-difference-between-logistic-regression-and-Naive-Bayes</t>
+  </si>
+  <si>
+    <t>#Why bayesGLM seems better?</t>
   </si>
 </sst>
 </file>
@@ -128,7 +134,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -136,6 +142,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E905E9D4-D440-4A8A-92B2-D022498CC8E2}">
-  <dimension ref="B3:G12"/>
+  <dimension ref="B3:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -691,6 +698,16 @@
         <v>0.23579549999999999</v>
       </c>
     </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B15" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B16" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added cross validation error for each knn model
</commit_message>
<xml_diff>
--- a/summaryVotePredictionModels.xlsx
+++ b/summaryVotePredictionModels.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7990" activeTab="1" xr2:uid="{11D3DAA1-BD6D-43CE-B66A-90E4F359C9CA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7990" xr2:uid="{11D3DAA1-BD6D-43CE-B66A-90E4F359C9CA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="knn class" sheetId="1" r:id="rId1"/>
     <sheet name="caret" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
   <si>
     <t>Sensitivity Rate of True Positives</t>
   </si>
@@ -33,75 +33,12 @@
     <t>Sensibility Rate of True Negatives</t>
   </si>
   <si>
-    <t>Naïve Bayes</t>
-  </si>
-  <si>
-    <t>k-Nearest Neighborhood</t>
-  </si>
-  <si>
-    <t>SVM</t>
-  </si>
-  <si>
-    <t>Random Forest</t>
-  </si>
-  <si>
-    <t>Generalized Linear Model</t>
-  </si>
-  <si>
-    <t>method</t>
-  </si>
-  <si>
-    <t>nb</t>
-  </si>
-  <si>
-    <t>rf</t>
-  </si>
-  <si>
-    <t>glm</t>
-  </si>
-  <si>
-    <t>hyperparameters</t>
-  </si>
-  <si>
     <t>model</t>
   </si>
   <si>
-    <t>knn</t>
-  </si>
-  <si>
     <t>ROC AUC (Receiver Operator Curve Area Under the Curve)</t>
   </si>
   <si>
-    <t>TRUE class</t>
-  </si>
-  <si>
-    <t>FALSE class</t>
-  </si>
-  <si>
-    <t>bayesglm</t>
-  </si>
-  <si>
-    <t>svmLinear</t>
-  </si>
-  <si>
-    <t>svmLinear2</t>
-  </si>
-  <si>
-    <t>cost=0.5</t>
-  </si>
-  <si>
-    <t>svmLinearWeights</t>
-  </si>
-  <si>
-    <t>cost=0.5, weight=3</t>
-  </si>
-  <si>
-    <t>https://www.quora.com/What-is-the-difference-between-logistic-regression-and-Naive-Bayes</t>
-  </si>
-  <si>
-    <t>#Why bayesGLM seems better?</t>
-  </si>
-  <si>
     <t>GLM</t>
   </si>
   <si>
@@ -127,14 +64,92 @@
   </si>
   <si>
     <t>2, 3, 2, 2, 2, 2</t>
+  </si>
+  <si>
+    <t>True Positives</t>
+  </si>
+  <si>
+    <t>False Positives</t>
+  </si>
+  <si>
+    <t>False Negatives</t>
+  </si>
+  <si>
+    <t>True Negatives</t>
+  </si>
+  <si>
+    <t>K-Nearest Neighbor with leave-one-out cross validation</t>
+  </si>
+  <si>
+    <t>accuracy</t>
+  </si>
+  <si>
+    <t>Ranking</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>cross-validation error</t>
+  </si>
+  <si>
+    <t>Aggregation mechanism</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>AM.1</t>
+  </si>
+  <si>
+    <t>AM.2</t>
+  </si>
+  <si>
+    <t>AM.3</t>
+  </si>
+  <si>
+    <t>AM.3 RANKING</t>
+  </si>
+  <si>
+    <t>AM.1 THRESHOLD</t>
+  </si>
+  <si>
+    <t>AM.2 MAJORITY VOTE</t>
+  </si>
+  <si>
+    <t>generalization error</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -159,10 +174,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -174,21 +190,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="41">
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -198,6 +232,30 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -220,6 +278,57 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -238,35 +347,92 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{26070705-A123-4DA7-96C0-32A5815261E3}" name="Table1" displayName="Table1" ref="B3:G12" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="B3:G12" xr:uid="{A438C972-3F10-41AC-9D4F-3C567B3CDCDC}"/>
-  <sortState ref="B4:G12">
-    <sortCondition descending="1" ref="E3:E12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{26070705-A123-4DA7-96C0-32A5815261E3}" name="Table1" displayName="Table1" ref="B3:H10" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+  <autoFilter ref="B3:H10" xr:uid="{A438C972-3F10-41AC-9D4F-3C567B3CDCDC}"/>
+  <sortState ref="B4:G10">
+    <sortCondition ref="C3:C10"/>
   </sortState>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{BA26ADEE-92F6-4283-84A8-2EBE482B549A}" name="model" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{7FC6B75C-6DEC-412C-852B-D951599F8439}" name="method" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{ABE7CF55-0C6C-4D4C-A2E3-374E40F23289}" name="hyperparameters" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{60495A30-3957-41A1-963D-2FA95354A629}" name="ROC AUC (Receiver Operator Curve Area Under the Curve)" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{2323F2B2-90F6-4C03-9AA7-176E30E5EA99}" name="Sensitivity Rate of True Positives" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{3A32E282-2981-4384-AAB1-D3BBC6636D3B}" name="Sensibility Rate of True Negatives" dataDxfId="7"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{BA26ADEE-92F6-4283-84A8-2EBE482B549A}" name="model" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{ABE7CF55-0C6C-4D4C-A2E3-374E40F23289}" name="accuracy" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{60495A30-3957-41A1-963D-2FA95354A629}" name="True Positives" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{2323F2B2-90F6-4C03-9AA7-176E30E5EA99}" name="True Negatives" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{3A32E282-2981-4384-AAB1-D3BBC6636D3B}" name="False Positives" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{9CD4AB14-A737-46B6-9617-891C27247FFB}" name="False Negatives" dataDxfId="17"/>
+    <tableColumn id="8" xr3:uid="{16FF2B99-8F06-4611-9A48-1C7FCDC36F95}" name="Ranking" dataDxfId="16"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{715B3029-2E91-41C9-BD8D-DF96ACD38759}" name="Table14" displayName="Table14" ref="B14:H18" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+  <autoFilter ref="B14:H18" xr:uid="{E4FE1238-E632-4650-8E8F-A11930E40BBF}"/>
+  <sortState ref="B15:G18">
+    <sortCondition ref="C3:C10"/>
+  </sortState>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{1E735F1D-CDF3-40FD-AE1D-382DD93495CB}" name="model" dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{1763246E-7C47-47DE-A72B-D1EA8634513C}" name="accuracy" dataDxfId="30">
+      <calculatedColumnFormula>SUM(Table14[[#This Row],[True Positives]:[True Negatives]])/SUM(Table14[[#This Row],[True Positives]:[False Negatives]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{54093B99-6537-40A4-B903-C0A753464B04}" name="True Positives" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{4C3E7059-3322-4869-BBB9-285761E56FE2}" name="True Negatives" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{CD18F6DE-FF92-4534-B41A-292D55A4207C}" name="False Positives" dataDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{0669E59D-03FB-4922-BE05-208C9221EDD0}" name="False Negatives" dataDxfId="26"/>
+    <tableColumn id="8" xr3:uid="{1E4BF6AD-99C2-479B-9F80-DDB3CB63314C}" name="Threshold" dataDxfId="25"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{798D58E5-800D-4FD4-9E2F-BE951676B373}" name="Table145" displayName="Table145" ref="B22:H26" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="B22:H26" xr:uid="{80AEDBD2-DBB0-45F9-9D36-2E600C16E540}"/>
+  <sortState ref="B23:G26">
+    <sortCondition ref="C3:C10"/>
+  </sortState>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{AC864E6D-8E88-44B1-B2CD-078850D9C0C2}" name="model" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{F1A902D5-5525-4F6B-BB51-B577BC3BD560}" name="accuracy" dataDxfId="12">
+      <calculatedColumnFormula>SUM(Table145[[#This Row],[True Positives]:[True Negatives]])/SUM(Table145[[#This Row],[True Positives]:[False Negatives]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{D8E42556-2752-4020-A5A2-C34F1B365E5B}" name="True Positives" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{7A2BA5DC-5762-4069-ABAF-1548014E1D14}" name="True Negatives" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{22FBECAE-4DDE-4AFA-9C3F-DB9E683A9A2B}" name="False Positives" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{CB14F0E6-2F97-4C94-907D-5B473F04B319}" name="False Negatives" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{2B947D44-3F7F-46B9-887B-B617634ADD7E}" name="Threshold" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{25483E7F-88A1-4D45-A3DB-8811E9379E40}" name="Table13" displayName="Table13" ref="B3:F9" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{70BD5F80-DC43-4179-B4CA-F459FC673450}" name="Table5" displayName="Table5" ref="B29:F32" totalsRowShown="0" headerRowDxfId="1" dataDxfId="2">
+  <autoFilter ref="B29:F32" xr:uid="{2E41160F-3EAF-48EF-A1E5-3A508AB6C2B6}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{89CDDEF4-2006-4CC2-8702-01D97ECD9FFE}" name="Aggregation mechanism" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{6F94AF4C-FE23-48EC-9CA2-82AD7DA29C2D}" name="k" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{1933BB4F-EFD7-44A6-A26C-AA85293D75AB}" name="cross-validation error" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{BE494206-5029-4AF8-8FF9-0751AB91C87B}" name="n" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{348B0B88-6665-4983-BAB7-C91E9E335308}" name="generalization error" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{25483E7F-88A1-4D45-A3DB-8811E9379E40}" name="Table13" displayName="Table13" ref="B3:F9" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
   <autoFilter ref="B3:F9" xr:uid="{4EE24B2E-1496-4E1A-AD27-C2647F430286}"/>
   <sortState ref="B4:F9">
     <sortCondition ref="E3:E9"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="6" xr3:uid="{74D2DE9A-B30C-484D-BE41-296992A34AA9}" name="number of folds (k)" dataDxfId="4"/>
-    <tableColumn id="1" xr3:uid="{601B47CC-1D66-4216-BF9B-E9E4FF81F454}" name="Samples and sizes" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{3B6C7B2A-86F8-4582-9227-83370F3B25F7}" name="ROC AUC (Receiver Operator Curve Area Under the Curve)" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{D4A7C258-516A-4C68-B14F-A507710EFE7B}" name="Sensitivity Rate of True Positives" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{2FF3F640-5070-4972-B3F6-0ACEF875EE92}" name="Sensibility Rate of True Negatives" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{74D2DE9A-B30C-484D-BE41-296992A34AA9}" name="number of folds (k)" dataDxfId="38"/>
+    <tableColumn id="1" xr3:uid="{601B47CC-1D66-4216-BF9B-E9E4FF81F454}" name="Samples and sizes" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{3B6C7B2A-86F8-4582-9227-83370F3B25F7}" name="ROC AUC (Receiver Operator Curve Area Under the Curve)" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{D4A7C258-516A-4C68-B14F-A507710EFE7B}" name="Sensitivity Rate of True Positives" dataDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{2FF3F640-5070-4972-B3F6-0ACEF875EE92}" name="Sensibility Rate of True Negatives" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -569,219 +735,571 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E905E9D4-D440-4A8A-92B2-D022498CC8E2}">
-  <dimension ref="B3:G16"/>
+  <dimension ref="B1:H32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37:D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.36328125" style="1" customWidth="1"/>
     <col min="2" max="2" width="23.54296875" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="17.90625" style="1"/>
+    <col min="3" max="3" width="17.90625" style="1"/>
+    <col min="4" max="4" width="20.7265625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="17.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B1" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="8">
+        <f>1-C4</f>
+        <v>6.2015503875968991E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="23" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <f>SUM(Table1[[#This Row],[True Positives]:[True Negatives]])/SUM(Table1[[#This Row],[True Positives]:[False Negatives]])</f>
+        <v>0.93798449612403101</v>
+      </c>
+      <c r="D4" s="1">
+        <v>102</v>
+      </c>
+      <c r="E4" s="1">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>6</v>
+      </c>
+      <c r="H4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B5" s="1">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1">
+        <f>SUM(Table1[[#This Row],[True Positives]:[True Negatives]])/SUM(Table1[[#This Row],[True Positives]:[False Negatives]])</f>
+        <v>0.93798449612403101</v>
+      </c>
+      <c r="D5" s="1">
+        <v>102</v>
+      </c>
+      <c r="E5" s="1">
+        <v>19</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>6</v>
+      </c>
+      <c r="H5" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B6" s="1">
         <v>7</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="C6" s="1">
+        <f>SUM(Table1[[#This Row],[True Positives]:[True Negatives]])/SUM(Table1[[#This Row],[True Positives]:[False Negatives]])</f>
+        <v>0.93798449612403101</v>
+      </c>
+      <c r="D6" s="1">
+        <v>102</v>
+      </c>
+      <c r="E6" s="1">
+        <v>19</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>6</v>
+      </c>
+      <c r="H6" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B7" s="1">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1">
+        <f>SUM(Table1[[#This Row],[True Positives]:[True Negatives]])/SUM(Table1[[#This Row],[True Positives]:[False Negatives]])</f>
+        <v>0.93798449612403101</v>
+      </c>
+      <c r="D7" s="1">
+        <v>102</v>
+      </c>
+      <c r="E7" s="1">
+        <v>19</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>6</v>
+      </c>
+      <c r="H7" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B8" s="1">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1">
+        <f>SUM(Table1[[#This Row],[True Positives]:[True Negatives]])/SUM(Table1[[#This Row],[True Positives]:[False Negatives]])</f>
+        <v>0.93798449612403101</v>
+      </c>
+      <c r="D8" s="1">
+        <v>102</v>
+      </c>
+      <c r="E8" s="1">
+        <v>19</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1">
+        <v>6</v>
+      </c>
+      <c r="H8" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B9" s="1">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1">
+        <f>SUM(Table1[[#This Row],[True Positives]:[True Negatives]])/SUM(Table1[[#This Row],[True Positives]:[False Negatives]])</f>
+        <v>0.96124031007751942</v>
+      </c>
+      <c r="D9" s="1">
+        <v>102</v>
+      </c>
+      <c r="E9" s="1">
+        <v>22</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1">
+        <v>3</v>
+      </c>
+      <c r="H9" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
+        <f>SUM(Table1[[#This Row],[True Positives]:[True Negatives]])/SUM(Table1[[#This Row],[True Positives]:[False Negatives]])</f>
+        <v>0.99224806201550386</v>
+      </c>
+      <c r="D10" s="1">
+        <v>104</v>
+      </c>
+      <c r="E10" s="1">
+        <v>24</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B12" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="6">
+        <f>1-C15</f>
+        <v>2.3255813953488413E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="G14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B15" s="1">
+        <v>3</v>
+      </c>
+      <c r="C15" s="1">
+        <f>SUM(Table14[[#This Row],[True Positives]:[True Negatives]])/SUM(Table14[[#This Row],[True Positives]:[False Negatives]])</f>
+        <v>0.97674418604651159</v>
+      </c>
+      <c r="D15" s="1">
+        <v>103</v>
+      </c>
+      <c r="E15" s="1">
+        <v>23</v>
+      </c>
+      <c r="F15" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="2:7" ht="23" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="1" t="s">
+      <c r="G15" s="1">
+        <v>2</v>
+      </c>
+      <c r="H15" s="1">
         <v>6</v>
       </c>
-      <c r="C4" s="1" t="s">
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B16" s="1">
+        <v>5</v>
+      </c>
+      <c r="C16" s="1">
+        <f>SUM(Table14[[#This Row],[True Positives]:[True Negatives]])/SUM(Table14[[#This Row],[True Positives]:[False Negatives]])</f>
+        <v>0.93023255813953487</v>
+      </c>
+      <c r="D16" s="1">
+        <v>103</v>
+      </c>
+      <c r="E16" s="1">
         <v>17</v>
       </c>
-      <c r="E4" s="1">
-        <v>0.8898239</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0.93229320000000004</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0.43710139999999997</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B5" s="1" t="s">
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <v>8</v>
+      </c>
+      <c r="H16" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B17" s="1">
+        <v>7</v>
+      </c>
+      <c r="C17" s="1">
+        <f>SUM(Table14[[#This Row],[True Positives]:[True Negatives]])/SUM(Table14[[#This Row],[True Positives]:[False Negatives]])</f>
+        <v>0.93023255813953487</v>
+      </c>
+      <c r="D17" s="1">
+        <v>103</v>
+      </c>
+      <c r="E17" s="1">
+        <v>17</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1">
+        <v>8</v>
+      </c>
+      <c r="H17" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B18" s="1">
+        <v>9</v>
+      </c>
+      <c r="C18" s="1">
+        <f>SUM(Table14[[#This Row],[True Positives]:[True Negatives]])/SUM(Table14[[#This Row],[True Positives]:[False Negatives]])</f>
+        <v>0.9147286821705426</v>
+      </c>
+      <c r="D18" s="1">
+        <v>99</v>
+      </c>
+      <c r="E18" s="1">
+        <v>19</v>
+      </c>
+      <c r="F18" s="1">
+        <v>5</v>
+      </c>
+      <c r="G18" s="1">
         <v>6</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="H18" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B20" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="8">
+        <f>1-C23</f>
+        <v>0.12403100775193798</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B23" s="1">
+        <v>3</v>
+      </c>
+      <c r="C23" s="1">
+        <f>SUM(Table145[[#This Row],[True Positives]:[True Negatives]])/SUM(Table145[[#This Row],[True Positives]:[False Negatives]])</f>
+        <v>0.87596899224806202</v>
+      </c>
+      <c r="D23" s="1">
+        <v>98</v>
+      </c>
+      <c r="E23" s="1">
+        <v>15</v>
+      </c>
+      <c r="F23" s="1">
+        <v>6</v>
+      </c>
+      <c r="G23" s="1">
         <v>10</v>
       </c>
-      <c r="E5" s="1">
-        <v>0.87471129999999997</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0.92378260000000001</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0.45073780000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B6" s="1" t="s">
+      <c r="H23" s="1">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B24" s="1">
+        <v>5</v>
+      </c>
+      <c r="C24" s="1">
+        <f>SUM(Table145[[#This Row],[True Positives]:[True Negatives]])/SUM(Table145[[#This Row],[True Positives]:[False Negatives]])</f>
+        <v>0.87596899224806202</v>
+      </c>
+      <c r="D24" s="1">
+        <v>98</v>
+      </c>
+      <c r="E24" s="1">
+        <v>15</v>
+      </c>
+      <c r="F24" s="1">
+        <v>6</v>
+      </c>
+      <c r="G24" s="1">
+        <v>10</v>
+      </c>
+      <c r="H24" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B25" s="1">
+        <v>7</v>
+      </c>
+      <c r="C25" s="1">
+        <f>SUM(Table145[[#This Row],[True Positives]:[True Negatives]])/SUM(Table145[[#This Row],[True Positives]:[False Negatives]])</f>
+        <v>0.87596899224806202</v>
+      </c>
+      <c r="D25" s="1">
+        <v>98</v>
+      </c>
+      <c r="E25" s="1">
+        <v>15</v>
+      </c>
+      <c r="F25" s="1">
+        <v>6</v>
+      </c>
+      <c r="G25" s="1">
+        <v>10</v>
+      </c>
+      <c r="H25" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B26" s="1">
+        <v>9</v>
+      </c>
+      <c r="C26" s="1">
+        <f>SUM(Table145[[#This Row],[True Positives]:[True Negatives]])/SUM(Table145[[#This Row],[True Positives]:[False Negatives]])</f>
+        <v>0.87596899224806202</v>
+      </c>
+      <c r="D26" s="1">
+        <v>98</v>
+      </c>
+      <c r="E26" s="1">
+        <v>15</v>
+      </c>
+      <c r="F26" s="1">
+        <v>6</v>
+      </c>
+      <c r="G26" s="1">
+        <v>10</v>
+      </c>
+      <c r="H26" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B29" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B30" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="4">
         <v>3</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0.82901369999999996</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0.97789470000000001</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0.13409090000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0.81245449999999997</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0.87628760000000006</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0.51322460000000003</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0.81026790000000004</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0.84391139999999998</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0.5645059</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0.77135659999999995</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0.9757671</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0.1613636</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0.75469699999999995</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0.90314090000000002</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0.56645959999999995</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0.75345379999999995</v>
-      </c>
-      <c r="F11" s="1">
-        <v>0.92704839999999999</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0.50951089999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0.67986179999999996</v>
-      </c>
-      <c r="F12" s="1">
-        <v>0.96438970000000002</v>
-      </c>
-      <c r="G12" s="1">
-        <v>0.23579549999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B15" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B16" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="D30" s="9">
+        <f>C13</f>
+        <v>2.3255813953488413E-2</v>
+      </c>
+      <c r="E30" s="4">
+        <v>6</v>
+      </c>
+      <c r="F30" s="4"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B31" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="4">
+        <v>3</v>
+      </c>
+      <c r="D31" s="9">
+        <f>C21</f>
+        <v>0.12403100775193798</v>
+      </c>
+      <c r="E31" s="4">
+        <v>-2</v>
+      </c>
+      <c r="F31" s="4"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B32" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="4">
+        <v>3</v>
+      </c>
+      <c r="D32" s="9">
+        <f>D2</f>
+        <v>6.2015503875968991E-2</v>
+      </c>
+      <c r="E32" s="4">
+        <v>3</v>
+      </c>
+      <c r="F32" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
+  <tableParts count="4">
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
@@ -790,7 +1308,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{103C3932-7911-4558-8622-359D7BC2E5F7}">
   <dimension ref="B2:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -806,18 +1324,18 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>0</v>
@@ -831,7 +1349,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D4" s="4">
         <v>0.59894179999999997</v>
@@ -848,7 +1366,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D5" s="4">
         <v>0.59659859999999998</v>
@@ -865,7 +1383,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="D6" s="4">
         <v>0.78854170000000001</v>
@@ -882,7 +1400,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D7" s="4">
         <v>0.89880950000000004</v>
@@ -899,7 +1417,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="D8" s="4">
         <v>0.88452379999999997</v>
@@ -916,7 +1434,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="D9" s="4">
         <v>0.95</v>

</xml_diff>

<commit_message>
summary of kFold charts
</commit_message>
<xml_diff>
--- a/summaryVotePredictionModels.xlsx
+++ b/summaryVotePredictionModels.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="44">
   <si>
     <t>Sensitivity Rate of True Positives</t>
   </si>
@@ -158,6 +158,9 @@
   </si>
   <si>
     <t>True positive rate x False positive rate</t>
+  </si>
+  <si>
+    <t>As folds increase, the false positives decrease, which is overfitting, because the algorithm took False as the positive class</t>
   </si>
 </sst>
 </file>
@@ -1056,10 +1059,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'kfold-svm'!$B$4:$B$24</c:f>
+              <c:f>'kfold-svm'!$B$4:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -1112,15 +1115,18 @@
                   <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>75</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>90</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>115</c:v>
                 </c:pt>
               </c:numCache>
@@ -1128,10 +1134,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'kfold-svm'!$C$4:$C$24</c:f>
+              <c:f>'kfold-svm'!$C$4:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>0.86281620000000003</c:v>
                 </c:pt>
@@ -1184,15 +1190,18 @@
                   <c:v>0.41639979999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>0.36906610000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>0.42305809999999999</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>0.41728539999999997</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>0.43499539999999998</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>0.4523182</c:v>
                 </c:pt>
               </c:numCache>
@@ -1638,10 +1647,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'kfold-svm'!$B$4:$B$24</c:f>
+              <c:f>'kfold-svm'!$B$4:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -1694,15 +1703,18 @@
                   <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>75</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>90</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>115</c:v>
                 </c:pt>
               </c:numCache>
@@ -1710,10 +1722,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'kfold-svm'!$E$4:$E$24</c:f>
+              <c:f>'kfold-svm'!$E$4:$E$25</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>0.3333333</c:v>
                 </c:pt>
@@ -1766,15 +1778,18 @@
                   <c:v>0.62639990000000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>0.69246030000000003</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>0.61979169999999995</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>0.76515149999999998</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>0.80952380000000002</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>0.83333330000000005</c:v>
                 </c:pt>
               </c:numCache>
@@ -2221,10 +2236,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'kfold-svm'!$B$4:$B$24</c:f>
+              <c:f>'kfold-svm'!$B$4:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -2277,15 +2292,18 @@
                   <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>75</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>90</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>115</c:v>
                 </c:pt>
               </c:numCache>
@@ -2293,10 +2311,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'kfold-svm'!$D$4:$D$24</c:f>
+              <c:f>'kfold-svm'!$D$4:$D$25</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>0.90178570000000002</c:v>
                 </c:pt>
@@ -2349,15 +2367,18 @@
                   <c:v>0.67998369999999997</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>0.79657880000000003</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>0.67293689000000001</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>0.77228600000000003</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>0.7337032</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>0.71359220000000001</c:v>
                 </c:pt>
               </c:numCache>
@@ -15273,7 +15294,7 @@
   <dimension ref="B3:F23"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19:D23"/>
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16101,10 +16122,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5CE95F2-2905-4F40-965A-C017CDB146E7}">
-  <dimension ref="B3:E31"/>
+  <dimension ref="B3:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24:O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16309,7 +16330,7 @@
         <v>0.37009730000000002</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B17" s="11">
         <v>15</v>
       </c>
@@ -16323,7 +16344,7 @@
         <v>0.63246990000000003</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B18" s="11">
         <v>30</v>
       </c>
@@ -16337,7 +16358,7 @@
         <v>0.72826089999999999</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B19" s="11">
         <v>45</v>
       </c>
@@ -16351,7 +16372,7 @@
         <v>0.497807</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B20" s="11">
         <v>60</v>
       </c>
@@ -16364,100 +16385,117 @@
       <c r="E20" s="13">
         <v>0.62639990000000001</v>
       </c>
+      <c r="O20" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B21" s="11">
+        <v>70</v>
+      </c>
+      <c r="C21" s="13">
+        <v>0.36906610000000001</v>
+      </c>
+      <c r="D21" s="13">
+        <v>0.79657880000000003</v>
+      </c>
+      <c r="E21" s="13">
+        <v>0.69246030000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B22" s="11">
         <v>75</v>
       </c>
-      <c r="C21" s="13">
+      <c r="C22" s="13">
         <v>0.42305809999999999</v>
       </c>
-      <c r="D21" s="13">
+      <c r="D22" s="13">
         <v>0.67293689000000001</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E22" s="13">
         <v>0.61979169999999995</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B22" s="11">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B23" s="11">
         <v>90</v>
       </c>
-      <c r="C22" s="13">
+      <c r="C23" s="13">
         <v>0.41728539999999997</v>
       </c>
-      <c r="D22" s="13">
+      <c r="D23" s="13">
         <v>0.77228600000000003</v>
       </c>
-      <c r="E22" s="13">
+      <c r="E23" s="13">
         <v>0.76515149999999998</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B23" s="11">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B24" s="11">
         <v>100</v>
       </c>
-      <c r="C23" s="13">
+      <c r="C24" s="13">
         <v>0.43499539999999998</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D24" s="13">
         <v>0.7337032</v>
       </c>
-      <c r="E23" s="13">
+      <c r="E24" s="13">
         <v>0.80952380000000002</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B24" s="11">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B25" s="11">
         <v>115</v>
       </c>
-      <c r="C24" s="13">
+      <c r="C25" s="13">
         <v>0.4523182</v>
       </c>
-      <c r="D24" s="13">
+      <c r="D25" s="13">
         <v>0.71359220000000001</v>
       </c>
-      <c r="E24" s="13">
+      <c r="E25" s="13">
         <v>0.83333330000000005</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B26" t="s">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
         <v>35</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B27" t="s">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
         <v>36</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B28" t="s">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
         <v>37</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B30" t="s">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
         <v>36</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B31" t="s">
+    <row r="32" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
         <v>37</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed number of folds
</commit_message>
<xml_diff>
--- a/summaryVotePredictionModels.xlsx
+++ b/summaryVotePredictionModels.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,15 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7990" activeTab="5" xr2:uid="{11D3DAA1-BD6D-43CE-B66A-90E4F359C9CA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7990" xr2:uid="{11D3DAA1-BD6D-43CE-B66A-90E4F359C9CA}"/>
   </bookViews>
   <sheets>
-    <sheet name="knn class" sheetId="1" r:id="rId1"/>
-    <sheet name="caret" sheetId="2" r:id="rId2"/>
-    <sheet name="kfold-knn" sheetId="3" r:id="rId3"/>
-    <sheet name="kfold-rf" sheetId="4" r:id="rId4"/>
-    <sheet name="kfold-glm" sheetId="5" r:id="rId5"/>
-    <sheet name="kfold-svm" sheetId="6" r:id="rId6"/>
+    <sheet name="models" sheetId="7" r:id="rId1"/>
+    <sheet name="knn class" sheetId="1" r:id="rId2"/>
+    <sheet name="caret" sheetId="2" r:id="rId3"/>
+    <sheet name="kfold-knn" sheetId="3" r:id="rId4"/>
+    <sheet name="kfold-rf" sheetId="4" r:id="rId5"/>
+    <sheet name="kfold-glm" sheetId="5" r:id="rId6"/>
+    <sheet name="kfold-svm" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="67">
   <si>
     <t>Sensitivity Rate of True Positives</t>
   </si>
@@ -162,6 +163,75 @@
   <si>
     <t>As folds increase, the false positives decrease, which is overfitting, because the algorithm took False as the positive class</t>
   </si>
+  <si>
+    <t>AUC</t>
+  </si>
+  <si>
+    <t>specificity</t>
+  </si>
+  <si>
+    <t>sensitivity</t>
+  </si>
+  <si>
+    <t>10-fold cross-validation</t>
+  </si>
+  <si>
+    <t>bayes GLM</t>
+  </si>
+  <si>
+    <t>SVM Linear2</t>
+  </si>
+  <si>
+    <t>glm</t>
+  </si>
+  <si>
+    <t>naïve bayes</t>
+  </si>
+  <si>
+    <t>random forest</t>
+  </si>
+  <si>
+    <t>Training Error</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>Recall</t>
+  </si>
+  <si>
+    <t>Model name</t>
+  </si>
+  <si>
+    <t>svm linear</t>
+  </si>
+  <si>
+    <t>svm linear weights</t>
+  </si>
+  <si>
+    <t>Training error consists of the complement of the accuracy, which was obtained during training, i.e., it did not use a third data set. That would be the validation error.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The table is sorted in descending order of Precision, which ranked random forest at top. This choice prioritizes the minimization of false positives. </t>
+  </si>
+  <si>
+    <t>If we would like to minimize the number of false negatives, we would chose svm linear weights instead. That could be the case when we are more concerned with  locating all faults, regardless of the cost of having to inspect false positives.</t>
+  </si>
+  <si>
+    <t>All models however, gave the same predictions with regards to value of n for each of the three aggregation methods.</t>
+  </si>
+  <si>
+    <t>The value of n is computed by looking at the predictions and observing the value of their aggregation metrics.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No difference in AUC (area under the curve), which means that all methods produced equivalent predictions in terms of AUC equally.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">That was expected beause the methods were executed to optimize for Sensitivity (True Positives / (True Positives + False Negatives)) </t>
+  </si>
 </sst>
 </file>
 
@@ -170,7 +240,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,16 +269,30 @@
       <name val="Lucida Console"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor theme="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -216,12 +300,103 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -256,12 +431,116 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="41">
+  <dxfs count="54">
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -14175,92 +14454,115 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{26070705-A123-4DA7-96C0-32A5815261E3}" name="Table1" displayName="Table1" ref="B3:H10" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{93861009-02DA-4F10-9354-6FB82FA7E3A1}" name="Table6" displayName="Table6" ref="B3:M11" totalsRowShown="0" headerRowDxfId="12">
+  <sortState ref="B4:M11">
+    <sortCondition descending="1" ref="J3:J11"/>
+  </sortState>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{203ECC0F-E73C-455A-AE43-F8C71E1AAB51}" name="Model name" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{7F4C0035-DB0E-4BDB-AB53-7DC05AFC56E9}" name="Training Error" dataDxfId="10" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{3058EC86-C0D2-41AB-AAD9-A8654349141C}" name="AUC" dataDxfId="9" dataCellStyle="Percent"/>
+    <tableColumn id="4" xr3:uid="{09FE4FFB-B0F3-4560-B423-B6137B7BBD5C}" name="Accuracy" dataDxfId="8" dataCellStyle="Percent"/>
+    <tableColumn id="5" xr3:uid="{39F4951B-3426-4CAF-B951-7DC084CFC23C}" name="True Negatives" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{B777A813-AC3C-4CA9-97EF-83A2A334B803}" name="True Positives" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{A615AD21-BD62-4889-95F8-15AE55E53A02}" name="False Negatives" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{C37DC8B5-BC5C-4804-B4AF-7AA5D271729C}" name="False Positives" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{38245A90-7AA1-4017-AECC-A6E96FE092EB}" name="Precision" dataDxfId="3" dataCellStyle="Percent"/>
+    <tableColumn id="10" xr3:uid="{F7ACD116-5F1D-4E6B-8A4C-907FD0AE87C5}" name="Recall" dataDxfId="2" dataCellStyle="Percent"/>
+    <tableColumn id="11" xr3:uid="{CEE2D274-96C5-4E30-98FF-849C8CB34662}" name="sensitivity" dataDxfId="1" dataCellStyle="Percent"/>
+    <tableColumn id="12" xr3:uid="{F41DF220-52BF-4A14-82C0-B3F43CBF5545}" name="specificity" dataDxfId="0" dataCellStyle="Percent"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{26070705-A123-4DA7-96C0-32A5815261E3}" name="Table1" displayName="Table1" ref="B3:H10" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
   <autoFilter ref="B3:H10" xr:uid="{A438C972-3F10-41AC-9D4F-3C567B3CDCDC}"/>
   <sortState ref="B4:G10">
     <sortCondition ref="C3:C10"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{BA26ADEE-92F6-4283-84A8-2EBE482B549A}" name="model" dataDxfId="38"/>
-    <tableColumn id="6" xr3:uid="{ABE7CF55-0C6C-4D4C-A2E3-374E40F23289}" name="accuracy" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{60495A30-3957-41A1-963D-2FA95354A629}" name="True Positives" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{2323F2B2-90F6-4C03-9AA7-176E30E5EA99}" name="True Negatives" dataDxfId="35"/>
-    <tableColumn id="5" xr3:uid="{3A32E282-2981-4384-AAB1-D3BBC6636D3B}" name="False Positives" dataDxfId="34"/>
-    <tableColumn id="7" xr3:uid="{9CD4AB14-A737-46B6-9617-891C27247FFB}" name="False Negatives" dataDxfId="33"/>
-    <tableColumn id="8" xr3:uid="{16FF2B99-8F06-4611-9A48-1C7FCDC36F95}" name="Ranking" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{BA26ADEE-92F6-4283-84A8-2EBE482B549A}" name="model" dataDxfId="51"/>
+    <tableColumn id="6" xr3:uid="{ABE7CF55-0C6C-4D4C-A2E3-374E40F23289}" name="accuracy" dataDxfId="50"/>
+    <tableColumn id="3" xr3:uid="{60495A30-3957-41A1-963D-2FA95354A629}" name="True Positives" dataDxfId="49"/>
+    <tableColumn id="4" xr3:uid="{2323F2B2-90F6-4C03-9AA7-176E30E5EA99}" name="True Negatives" dataDxfId="48"/>
+    <tableColumn id="5" xr3:uid="{3A32E282-2981-4384-AAB1-D3BBC6636D3B}" name="False Positives" dataDxfId="47"/>
+    <tableColumn id="7" xr3:uid="{9CD4AB14-A737-46B6-9617-891C27247FFB}" name="False Negatives" dataDxfId="46"/>
+    <tableColumn id="8" xr3:uid="{16FF2B99-8F06-4611-9A48-1C7FCDC36F95}" name="Ranking" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{715B3029-2E91-41C9-BD8D-DF96ACD38759}" name="Table14" displayName="Table14" ref="B14:H18" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{715B3029-2E91-41C9-BD8D-DF96ACD38759}" name="Table14" displayName="Table14" ref="B14:H18" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
   <autoFilter ref="B14:H18" xr:uid="{E4FE1238-E632-4650-8E8F-A11930E40BBF}"/>
   <sortState ref="B15:G18">
     <sortCondition ref="C3:C10"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{1E735F1D-CDF3-40FD-AE1D-382DD93495CB}" name="model" dataDxfId="29"/>
-    <tableColumn id="6" xr3:uid="{1763246E-7C47-47DE-A72B-D1EA8634513C}" name="accuracy" dataDxfId="28">
+    <tableColumn id="1" xr3:uid="{1E735F1D-CDF3-40FD-AE1D-382DD93495CB}" name="model" dataDxfId="42"/>
+    <tableColumn id="6" xr3:uid="{1763246E-7C47-47DE-A72B-D1EA8634513C}" name="accuracy" dataDxfId="41">
       <calculatedColumnFormula>SUM(Table14[[#This Row],[True Positives]:[True Negatives]])/SUM(Table14[[#This Row],[True Positives]:[False Negatives]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{54093B99-6537-40A4-B903-C0A753464B04}" name="True Positives" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{4C3E7059-3322-4869-BBB9-285761E56FE2}" name="True Negatives" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{CD18F6DE-FF92-4534-B41A-292D55A4207C}" name="False Positives" dataDxfId="25"/>
-    <tableColumn id="7" xr3:uid="{0669E59D-03FB-4922-BE05-208C9221EDD0}" name="False Negatives" dataDxfId="24"/>
-    <tableColumn id="8" xr3:uid="{1E4BF6AD-99C2-479B-9F80-DDB3CB63314C}" name="Threshold" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{54093B99-6537-40A4-B903-C0A753464B04}" name="True Positives" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{4C3E7059-3322-4869-BBB9-285761E56FE2}" name="True Negatives" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{CD18F6DE-FF92-4534-B41A-292D55A4207C}" name="False Positives" dataDxfId="38"/>
+    <tableColumn id="7" xr3:uid="{0669E59D-03FB-4922-BE05-208C9221EDD0}" name="False Negatives" dataDxfId="37"/>
+    <tableColumn id="8" xr3:uid="{1E4BF6AD-99C2-479B-9F80-DDB3CB63314C}" name="Threshold" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{798D58E5-800D-4FD4-9E2F-BE951676B373}" name="Table145" displayName="Table145" ref="B22:H26" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{798D58E5-800D-4FD4-9E2F-BE951676B373}" name="Table145" displayName="Table145" ref="B22:H26" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="B22:H26" xr:uid="{80AEDBD2-DBB0-45F9-9D36-2E600C16E540}"/>
   <sortState ref="B23:G26">
     <sortCondition ref="C3:C10"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{AC864E6D-8E88-44B1-B2CD-078850D9C0C2}" name="model" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{F1A902D5-5525-4F6B-BB51-B577BC3BD560}" name="accuracy" dataDxfId="19">
+    <tableColumn id="1" xr3:uid="{AC864E6D-8E88-44B1-B2CD-078850D9C0C2}" name="model" dataDxfId="33"/>
+    <tableColumn id="6" xr3:uid="{F1A902D5-5525-4F6B-BB51-B577BC3BD560}" name="accuracy" dataDxfId="32">
       <calculatedColumnFormula>SUM(Table145[[#This Row],[True Positives]:[True Negatives]])/SUM(Table145[[#This Row],[True Positives]:[False Negatives]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{D8E42556-2752-4020-A5A2-C34F1B365E5B}" name="True Positives" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{7A2BA5DC-5762-4069-ABAF-1548014E1D14}" name="True Negatives" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{22FBECAE-4DDE-4AFA-9C3F-DB9E683A9A2B}" name="False Positives" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{CB14F0E6-2F97-4C94-907D-5B473F04B319}" name="False Negatives" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{2B947D44-3F7F-46B9-887B-B617634ADD7E}" name="Threshold" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{D8E42556-2752-4020-A5A2-C34F1B365E5B}" name="True Positives" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{7A2BA5DC-5762-4069-ABAF-1548014E1D14}" name="True Negatives" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{22FBECAE-4DDE-4AFA-9C3F-DB9E683A9A2B}" name="False Positives" dataDxfId="29"/>
+    <tableColumn id="7" xr3:uid="{CB14F0E6-2F97-4C94-907D-5B473F04B319}" name="False Negatives" dataDxfId="28"/>
+    <tableColumn id="8" xr3:uid="{2B947D44-3F7F-46B9-887B-B617634ADD7E}" name="Threshold" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{70BD5F80-DC43-4179-B4CA-F459FC673450}" name="Table5" displayName="Table5" ref="B29:F32" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{70BD5F80-DC43-4179-B4CA-F459FC673450}" name="Table5" displayName="Table5" ref="B29:F32" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="B29:F32" xr:uid="{2E41160F-3EAF-48EF-A1E5-3A508AB6C2B6}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{89CDDEF4-2006-4CC2-8702-01D97ECD9FFE}" name="Aggregation mechanism" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{6F94AF4C-FE23-48EC-9CA2-82AD7DA29C2D}" name="k" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{1933BB4F-EFD7-44A6-A26C-AA85293D75AB}" name="cross-validation error" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{BE494206-5029-4AF8-8FF9-0751AB91C87B}" name="n" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{348B0B88-6665-4983-BAB7-C91E9E335308}" name="generalization error" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{89CDDEF4-2006-4CC2-8702-01D97ECD9FFE}" name="Aggregation mechanism" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{6F94AF4C-FE23-48EC-9CA2-82AD7DA29C2D}" name="k" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{1933BB4F-EFD7-44A6-A26C-AA85293D75AB}" name="cross-validation error" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{BE494206-5029-4AF8-8FF9-0751AB91C87B}" name="n" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{348B0B88-6665-4983-BAB7-C91E9E335308}" name="generalization error" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{25483E7F-88A1-4D45-A3DB-8811E9379E40}" name="Table13" displayName="Table13" ref="B3:F9" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{25483E7F-88A1-4D45-A3DB-8811E9379E40}" name="Table13" displayName="Table13" ref="B3:F9" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="B3:F9" xr:uid="{4EE24B2E-1496-4E1A-AD27-C2647F430286}"/>
   <sortState ref="B4:F9">
     <sortCondition ref="E3:E9"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="6" xr3:uid="{74D2DE9A-B30C-484D-BE41-296992A34AA9}" name="number of folds (k)" dataDxfId="4"/>
-    <tableColumn id="1" xr3:uid="{601B47CC-1D66-4216-BF9B-E9E4FF81F454}" name="Samples and sizes" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{3B6C7B2A-86F8-4582-9227-83370F3B25F7}" name="ROC AUC (Receiver Operator Curve Area Under the Curve)" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{D4A7C258-516A-4C68-B14F-A507710EFE7B}" name="Sensitivity Rate of True Positives" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{2FF3F640-5070-4972-B3F6-0ACEF875EE92}" name="Sensibility Rate of True Negatives" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{74D2DE9A-B30C-484D-BE41-296992A34AA9}" name="number of folds (k)" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{601B47CC-1D66-4216-BF9B-E9E4FF81F454}" name="Samples and sizes" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{3B6C7B2A-86F8-4582-9227-83370F3B25F7}" name="ROC AUC (Receiver Operator Curve Area Under the Curve)" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{D4A7C258-516A-4C68-B14F-A507710EFE7B}" name="Sensitivity Rate of True Positives" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{2FF3F640-5070-4972-B3F6-0ACEF875EE92}" name="Sensibility Rate of True Negatives" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -14562,10 +14864,423 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ECC3DC8-F219-4A35-9322-7470EB6D3D5C}">
+  <dimension ref="B2:M20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I21" sqref="H21:I21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="19.54296875" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="10.36328125" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" customWidth="1"/>
+    <col min="8" max="8" width="11.90625" customWidth="1"/>
+    <col min="9" max="9" width="10" customWidth="1"/>
+    <col min="10" max="10" width="10.36328125" customWidth="1"/>
+    <col min="12" max="12" width="11" customWidth="1"/>
+    <col min="13" max="13" width="11.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="B3" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="K3" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B4" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="20">
+        <v>0.124031007751938</v>
+      </c>
+      <c r="D4" s="20">
+        <v>0.74076923076923096</v>
+      </c>
+      <c r="E4" s="20">
+        <v>0.87596899224806202</v>
+      </c>
+      <c r="F4" s="21">
+        <v>100</v>
+      </c>
+      <c r="G4" s="21">
+        <v>13</v>
+      </c>
+      <c r="H4" s="21">
+        <v>12</v>
+      </c>
+      <c r="I4" s="21">
+        <v>4</v>
+      </c>
+      <c r="J4" s="20">
+        <v>0.76470588235294101</v>
+      </c>
+      <c r="K4" s="22">
+        <v>0.52</v>
+      </c>
+      <c r="L4" s="15">
+        <v>0.52</v>
+      </c>
+      <c r="M4" s="15">
+        <v>0.96153846153846201</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B5" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="20">
+        <v>0.124031007751938</v>
+      </c>
+      <c r="D5" s="20">
+        <v>0.74076923076923096</v>
+      </c>
+      <c r="E5" s="20">
+        <v>0.87596899224806202</v>
+      </c>
+      <c r="F5" s="21">
+        <v>99</v>
+      </c>
+      <c r="G5" s="21">
+        <v>14</v>
+      </c>
+      <c r="H5" s="21">
+        <v>11</v>
+      </c>
+      <c r="I5" s="21">
+        <v>5</v>
+      </c>
+      <c r="J5" s="20">
+        <v>0.73684210526315796</v>
+      </c>
+      <c r="K5" s="22">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="L5" s="15">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="M5" s="15">
+        <v>0.95192307692307698</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B6" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="20">
+        <v>0.13953488372093001</v>
+      </c>
+      <c r="D6" s="20">
+        <v>0.74076923076923096</v>
+      </c>
+      <c r="E6" s="20">
+        <v>0.86046511627906996</v>
+      </c>
+      <c r="F6" s="21">
+        <v>98</v>
+      </c>
+      <c r="G6" s="21">
+        <v>13</v>
+      </c>
+      <c r="H6" s="21">
+        <v>12</v>
+      </c>
+      <c r="I6" s="21">
+        <v>6</v>
+      </c>
+      <c r="J6" s="20">
+        <v>0.68421052631578905</v>
+      </c>
+      <c r="K6" s="22">
+        <v>0.52</v>
+      </c>
+      <c r="L6" s="15">
+        <v>0.52</v>
+      </c>
+      <c r="M6" s="15">
+        <v>0.94230769230769196</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B7" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="20">
+        <v>0.13953488372093001</v>
+      </c>
+      <c r="D7" s="20">
+        <v>0.74076923076923096</v>
+      </c>
+      <c r="E7" s="20">
+        <v>0.86046511627906996</v>
+      </c>
+      <c r="F7" s="21">
+        <v>98</v>
+      </c>
+      <c r="G7" s="21">
+        <v>13</v>
+      </c>
+      <c r="H7" s="21">
+        <v>12</v>
+      </c>
+      <c r="I7" s="21">
+        <v>6</v>
+      </c>
+      <c r="J7" s="20">
+        <v>0.68421052631578905</v>
+      </c>
+      <c r="K7" s="22">
+        <v>0.52</v>
+      </c>
+      <c r="L7" s="15">
+        <v>0.52</v>
+      </c>
+      <c r="M7" s="15">
+        <v>0.94230769230769196</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B8" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="20">
+        <v>0.13953488372093001</v>
+      </c>
+      <c r="D8" s="20">
+        <v>0.74076923076923096</v>
+      </c>
+      <c r="E8" s="20">
+        <v>0.86046511627906996</v>
+      </c>
+      <c r="F8" s="21">
+        <v>98</v>
+      </c>
+      <c r="G8" s="21">
+        <v>13</v>
+      </c>
+      <c r="H8" s="21">
+        <v>12</v>
+      </c>
+      <c r="I8" s="21">
+        <v>6</v>
+      </c>
+      <c r="J8" s="20">
+        <v>0.68421052631578905</v>
+      </c>
+      <c r="K8" s="22">
+        <v>0.52</v>
+      </c>
+      <c r="L8" s="15">
+        <v>0.52</v>
+      </c>
+      <c r="M8" s="15">
+        <v>0.94230769230769196</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B9" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="20">
+        <v>0.13953488372093001</v>
+      </c>
+      <c r="D9" s="20">
+        <v>0.74076923076923096</v>
+      </c>
+      <c r="E9" s="20">
+        <v>0.86046511627906996</v>
+      </c>
+      <c r="F9" s="21">
+        <v>98</v>
+      </c>
+      <c r="G9" s="21">
+        <v>13</v>
+      </c>
+      <c r="H9" s="21">
+        <v>12</v>
+      </c>
+      <c r="I9" s="21">
+        <v>6</v>
+      </c>
+      <c r="J9" s="20">
+        <v>0.68421052631578905</v>
+      </c>
+      <c r="K9" s="22">
+        <v>0.52</v>
+      </c>
+      <c r="L9" s="15">
+        <v>0.52</v>
+      </c>
+      <c r="M9" s="15">
+        <v>0.94230769230769196</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B10" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="20">
+        <v>0.162790697674419</v>
+      </c>
+      <c r="D10" s="20">
+        <v>0.74076923076923096</v>
+      </c>
+      <c r="E10" s="20">
+        <v>0.837209302325581</v>
+      </c>
+      <c r="F10" s="21">
+        <v>98</v>
+      </c>
+      <c r="G10" s="21">
+        <v>10</v>
+      </c>
+      <c r="H10" s="21">
+        <v>15</v>
+      </c>
+      <c r="I10" s="21">
+        <v>6</v>
+      </c>
+      <c r="J10" s="20">
+        <v>0.625</v>
+      </c>
+      <c r="K10" s="22">
+        <v>0.4</v>
+      </c>
+      <c r="L10" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="M10" s="15">
+        <v>0.94230769230769196</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="24">
+        <v>0.15503875968992301</v>
+      </c>
+      <c r="D11" s="24">
+        <v>0.74076923076923096</v>
+      </c>
+      <c r="E11" s="24">
+        <v>0.84496124031007702</v>
+      </c>
+      <c r="F11" s="25">
+        <v>90</v>
+      </c>
+      <c r="G11" s="25">
+        <v>19</v>
+      </c>
+      <c r="H11" s="25">
+        <v>6</v>
+      </c>
+      <c r="I11" s="25">
+        <v>14</v>
+      </c>
+      <c r="J11" s="24">
+        <v>0.57575757575757602</v>
+      </c>
+      <c r="K11" s="26">
+        <v>0.76</v>
+      </c>
+      <c r="L11" s="15">
+        <v>0.76</v>
+      </c>
+      <c r="M11" s="15">
+        <v>0.86538461538461497</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E905E9D4-D440-4A8A-92B2-D022498CC8E2}">
   <dimension ref="B1:H32"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D37" sqref="D37:D38"/>
     </sheetView>
   </sheetViews>
@@ -15132,12 +15847,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{103C3932-7911-4558-8622-359D7BC2E5F7}">
   <dimension ref="B2:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15289,7 +16004,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25AEB740-6AE2-4FAF-80AD-192013CED4F1}">
   <dimension ref="B3:F23"/>
   <sheetViews>
@@ -15596,7 +16311,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2C8D7A9-E1B8-40BF-BA41-272A23CF726B}">
   <dimension ref="B3:E26"/>
   <sheetViews>
@@ -15858,7 +16573,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19383C2D-EDF0-42FD-AA00-4CF79188BCEB}">
   <dimension ref="B3:E23"/>
   <sheetViews>
@@ -16120,12 +16835,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5CE95F2-2905-4F40-965A-C017CDB146E7}">
   <dimension ref="B3:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24:O28"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Explanation of the algorithm to learn the N (ranking, balance, threshold)
</commit_message>
<xml_diff>
--- a/summaryVotePredictionModels.xlsx
+++ b/summaryVotePredictionModels.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\OneDrive\Documentos\GitHub\ML_VotingAggregation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Documents\GitHub\ML_VotingAggregation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70942107-AF63-4E61-91B7-0506CD6117F2}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7990" xr2:uid="{11D3DAA1-BD6D-43CE-B66A-90E4F359C9CA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7988" activeTab="1" xr2:uid="{11D3DAA1-BD6D-43CE-B66A-90E4F359C9CA}"/>
   </bookViews>
   <sheets>
     <sheet name="models" sheetId="7" r:id="rId1"/>
-    <sheet name="knn class" sheetId="1" r:id="rId2"/>
-    <sheet name="caret" sheetId="2" r:id="rId3"/>
-    <sheet name="kfold-knn" sheetId="3" r:id="rId4"/>
-    <sheet name="kfold-rf" sheetId="4" r:id="rId5"/>
-    <sheet name="kfold-glm" sheetId="5" r:id="rId6"/>
-    <sheet name="kfold-svm" sheetId="6" r:id="rId7"/>
+    <sheet name="Summary" sheetId="8" r:id="rId2"/>
+    <sheet name="knn class" sheetId="1" r:id="rId3"/>
+    <sheet name="caret" sheetId="2" r:id="rId4"/>
+    <sheet name="kfold-knn" sheetId="3" r:id="rId5"/>
+    <sheet name="kfold-rf" sheetId="4" r:id="rId6"/>
+    <sheet name="kfold-glm" sheetId="5" r:id="rId7"/>
+    <sheet name="kfold-svm" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="86">
   <si>
     <t>Sensitivity Rate of True Positives</t>
   </si>
@@ -232,6 +234,84 @@
   <si>
     <t xml:space="preserve">That was expected beause the methods were executed to optimize for Sensitivity (True Positives / (True Positives + False Negatives)) </t>
   </si>
+  <si>
+    <t>To discover the value of N that minimizes the number of false negatives and false positives, we trained different machine learning methods.</t>
+  </si>
+  <si>
+    <t>arg min Precision(N) and arg min Recall(N)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Machine learning algorithms have several hypeparameters that influence the final prediction model. </t>
+  </si>
+  <si>
+    <t>Take for instance, the depth of the tree (Decision Trees), number of trees (Random Forest), number of kernels (KNN and SVM), etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To avoid arbitrary or trial and error determination of these hyperparameters, we adopted a library (caret [REF]) that </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Since we are dealing with </t>
+  </si>
+  <si>
+    <t>explores the hyperparameter space in a systematic way. This is done by optimizing the hyperparameter configuration that</t>
+  </si>
+  <si>
+    <t>maximize some metric, e.g., the area under the curve (AUC), which is a curve o true positive rate versus false positive rate.</t>
+  </si>
+  <si>
+    <t>a very imbalance dataset, we opted for the Precision Recall curve (PROC) instead.</t>
+  </si>
+  <si>
+    <r>
+      <t>[1]Davis, J., &amp; Goadrich, M. (2006, June). The relationship between Precision-Recall and ROC curves. In </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="5"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Proceedings of the 23rd international conference on Machine learning</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="5"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> (pp. 233-240). ACM.</t>
+    </r>
+  </si>
+  <si>
+    <t>PROC has been shown to work better for skewed datasets [1]</t>
+  </si>
+  <si>
+    <t>We used k-fold (k=10) cross-validation to train and test each model. On table-x we show the results for eight machine learning models.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The training error different from zero suggests that the models are not overfitting the training set. </t>
+  </si>
+  <si>
+    <t>We validated the models with at second dataset not used during the experiment. The errors are shown in table-Y.</t>
+  </si>
+  <si>
+    <t>Estimating N</t>
+  </si>
+  <si>
+    <t>We also validated this by making predictions on the hold-out dataset.</t>
+  </si>
+  <si>
+    <t>Threats to Validity</t>
+  </si>
+  <si>
+    <t>Write algorithm</t>
+  </si>
+  <si>
+    <t>We estimated N by taking the minimal value of N that would predict all bug-covering questions (ground truth).</t>
+  </si>
 </sst>
 </file>
 
@@ -240,7 +320,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -276,6 +356,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="5"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="5"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -396,7 +489,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -468,79 +561,13 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="54">
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -661,6 +688,73 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -14454,115 +14548,115 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{93861009-02DA-4F10-9354-6FB82FA7E3A1}" name="Table6" displayName="Table6" ref="B3:M11" totalsRowShown="0" headerRowDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{93861009-02DA-4F10-9354-6FB82FA7E3A1}" name="Table6" displayName="Table6" ref="B3:M11" totalsRowShown="0" headerRowDxfId="53">
   <sortState ref="B4:M11">
     <sortCondition descending="1" ref="J3:J11"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{203ECC0F-E73C-455A-AE43-F8C71E1AAB51}" name="Model name" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{7F4C0035-DB0E-4BDB-AB53-7DC05AFC56E9}" name="Training Error" dataDxfId="10" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{3058EC86-C0D2-41AB-AAD9-A8654349141C}" name="AUC" dataDxfId="9" dataCellStyle="Percent"/>
-    <tableColumn id="4" xr3:uid="{09FE4FFB-B0F3-4560-B423-B6137B7BBD5C}" name="Accuracy" dataDxfId="8" dataCellStyle="Percent"/>
-    <tableColumn id="5" xr3:uid="{39F4951B-3426-4CAF-B951-7DC084CFC23C}" name="True Negatives" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{B777A813-AC3C-4CA9-97EF-83A2A334B803}" name="True Positives" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{A615AD21-BD62-4889-95F8-15AE55E53A02}" name="False Negatives" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{C37DC8B5-BC5C-4804-B4AF-7AA5D271729C}" name="False Positives" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{38245A90-7AA1-4017-AECC-A6E96FE092EB}" name="Precision" dataDxfId="3" dataCellStyle="Percent"/>
-    <tableColumn id="10" xr3:uid="{F7ACD116-5F1D-4E6B-8A4C-907FD0AE87C5}" name="Recall" dataDxfId="2" dataCellStyle="Percent"/>
-    <tableColumn id="11" xr3:uid="{CEE2D274-96C5-4E30-98FF-849C8CB34662}" name="sensitivity" dataDxfId="1" dataCellStyle="Percent"/>
-    <tableColumn id="12" xr3:uid="{F41DF220-52BF-4A14-82C0-B3F43CBF5545}" name="specificity" dataDxfId="0" dataCellStyle="Percent"/>
+    <tableColumn id="1" xr3:uid="{203ECC0F-E73C-455A-AE43-F8C71E1AAB51}" name="Model name" dataDxfId="52"/>
+    <tableColumn id="2" xr3:uid="{7F4C0035-DB0E-4BDB-AB53-7DC05AFC56E9}" name="Training Error" dataDxfId="51" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{3058EC86-C0D2-41AB-AAD9-A8654349141C}" name="AUC" dataDxfId="50" dataCellStyle="Percent"/>
+    <tableColumn id="4" xr3:uid="{09FE4FFB-B0F3-4560-B423-B6137B7BBD5C}" name="Accuracy" dataDxfId="49" dataCellStyle="Percent"/>
+    <tableColumn id="5" xr3:uid="{39F4951B-3426-4CAF-B951-7DC084CFC23C}" name="True Negatives" dataDxfId="48"/>
+    <tableColumn id="6" xr3:uid="{B777A813-AC3C-4CA9-97EF-83A2A334B803}" name="True Positives" dataDxfId="47"/>
+    <tableColumn id="7" xr3:uid="{A615AD21-BD62-4889-95F8-15AE55E53A02}" name="False Negatives" dataDxfId="46"/>
+    <tableColumn id="8" xr3:uid="{C37DC8B5-BC5C-4804-B4AF-7AA5D271729C}" name="False Positives" dataDxfId="45"/>
+    <tableColumn id="9" xr3:uid="{38245A90-7AA1-4017-AECC-A6E96FE092EB}" name="Precision" dataDxfId="44" dataCellStyle="Percent"/>
+    <tableColumn id="10" xr3:uid="{F7ACD116-5F1D-4E6B-8A4C-907FD0AE87C5}" name="Recall" dataDxfId="43" dataCellStyle="Percent"/>
+    <tableColumn id="11" xr3:uid="{CEE2D274-96C5-4E30-98FF-849C8CB34662}" name="sensitivity" dataDxfId="42" dataCellStyle="Percent"/>
+    <tableColumn id="12" xr3:uid="{F41DF220-52BF-4A14-82C0-B3F43CBF5545}" name="specificity" dataDxfId="41" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{26070705-A123-4DA7-96C0-32A5815261E3}" name="Table1" displayName="Table1" ref="B3:H10" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{26070705-A123-4DA7-96C0-32A5815261E3}" name="Table1" displayName="Table1" ref="B3:H10" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
   <autoFilter ref="B3:H10" xr:uid="{A438C972-3F10-41AC-9D4F-3C567B3CDCDC}"/>
   <sortState ref="B4:G10">
     <sortCondition ref="C3:C10"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{BA26ADEE-92F6-4283-84A8-2EBE482B549A}" name="model" dataDxfId="51"/>
-    <tableColumn id="6" xr3:uid="{ABE7CF55-0C6C-4D4C-A2E3-374E40F23289}" name="accuracy" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{60495A30-3957-41A1-963D-2FA95354A629}" name="True Positives" dataDxfId="49"/>
-    <tableColumn id="4" xr3:uid="{2323F2B2-90F6-4C03-9AA7-176E30E5EA99}" name="True Negatives" dataDxfId="48"/>
-    <tableColumn id="5" xr3:uid="{3A32E282-2981-4384-AAB1-D3BBC6636D3B}" name="False Positives" dataDxfId="47"/>
-    <tableColumn id="7" xr3:uid="{9CD4AB14-A737-46B6-9617-891C27247FFB}" name="False Negatives" dataDxfId="46"/>
-    <tableColumn id="8" xr3:uid="{16FF2B99-8F06-4611-9A48-1C7FCDC36F95}" name="Ranking" dataDxfId="45"/>
+    <tableColumn id="1" xr3:uid="{BA26ADEE-92F6-4283-84A8-2EBE482B549A}" name="model" dataDxfId="38"/>
+    <tableColumn id="6" xr3:uid="{ABE7CF55-0C6C-4D4C-A2E3-374E40F23289}" name="accuracy" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{60495A30-3957-41A1-963D-2FA95354A629}" name="True Positives" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{2323F2B2-90F6-4C03-9AA7-176E30E5EA99}" name="True Negatives" dataDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{3A32E282-2981-4384-AAB1-D3BBC6636D3B}" name="False Positives" dataDxfId="34"/>
+    <tableColumn id="7" xr3:uid="{9CD4AB14-A737-46B6-9617-891C27247FFB}" name="False Negatives" dataDxfId="33"/>
+    <tableColumn id="8" xr3:uid="{16FF2B99-8F06-4611-9A48-1C7FCDC36F95}" name="Ranking" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{715B3029-2E91-41C9-BD8D-DF96ACD38759}" name="Table14" displayName="Table14" ref="B14:H18" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{715B3029-2E91-41C9-BD8D-DF96ACD38759}" name="Table14" displayName="Table14" ref="B14:H18" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
   <autoFilter ref="B14:H18" xr:uid="{E4FE1238-E632-4650-8E8F-A11930E40BBF}"/>
   <sortState ref="B15:G18">
     <sortCondition ref="C3:C10"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{1E735F1D-CDF3-40FD-AE1D-382DD93495CB}" name="model" dataDxfId="42"/>
-    <tableColumn id="6" xr3:uid="{1763246E-7C47-47DE-A72B-D1EA8634513C}" name="accuracy" dataDxfId="41">
+    <tableColumn id="1" xr3:uid="{1E735F1D-CDF3-40FD-AE1D-382DD93495CB}" name="model" dataDxfId="29"/>
+    <tableColumn id="6" xr3:uid="{1763246E-7C47-47DE-A72B-D1EA8634513C}" name="accuracy" dataDxfId="28">
       <calculatedColumnFormula>SUM(Table14[[#This Row],[True Positives]:[True Negatives]])/SUM(Table14[[#This Row],[True Positives]:[False Negatives]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{54093B99-6537-40A4-B903-C0A753464B04}" name="True Positives" dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{4C3E7059-3322-4869-BBB9-285761E56FE2}" name="True Negatives" dataDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{CD18F6DE-FF92-4534-B41A-292D55A4207C}" name="False Positives" dataDxfId="38"/>
-    <tableColumn id="7" xr3:uid="{0669E59D-03FB-4922-BE05-208C9221EDD0}" name="False Negatives" dataDxfId="37"/>
-    <tableColumn id="8" xr3:uid="{1E4BF6AD-99C2-479B-9F80-DDB3CB63314C}" name="Threshold" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{54093B99-6537-40A4-B903-C0A753464B04}" name="True Positives" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{4C3E7059-3322-4869-BBB9-285761E56FE2}" name="True Negatives" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{CD18F6DE-FF92-4534-B41A-292D55A4207C}" name="False Positives" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{0669E59D-03FB-4922-BE05-208C9221EDD0}" name="False Negatives" dataDxfId="24"/>
+    <tableColumn id="8" xr3:uid="{1E4BF6AD-99C2-479B-9F80-DDB3CB63314C}" name="Threshold" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{798D58E5-800D-4FD4-9E2F-BE951676B373}" name="Table145" displayName="Table145" ref="B22:H26" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{798D58E5-800D-4FD4-9E2F-BE951676B373}" name="Table145" displayName="Table145" ref="B22:H26" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
   <autoFilter ref="B22:H26" xr:uid="{80AEDBD2-DBB0-45F9-9D36-2E600C16E540}"/>
   <sortState ref="B23:G26">
     <sortCondition ref="C3:C10"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{AC864E6D-8E88-44B1-B2CD-078850D9C0C2}" name="model" dataDxfId="33"/>
-    <tableColumn id="6" xr3:uid="{F1A902D5-5525-4F6B-BB51-B577BC3BD560}" name="accuracy" dataDxfId="32">
+    <tableColumn id="1" xr3:uid="{AC864E6D-8E88-44B1-B2CD-078850D9C0C2}" name="model" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{F1A902D5-5525-4F6B-BB51-B577BC3BD560}" name="accuracy" dataDxfId="19">
       <calculatedColumnFormula>SUM(Table145[[#This Row],[True Positives]:[True Negatives]])/SUM(Table145[[#This Row],[True Positives]:[False Negatives]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{D8E42556-2752-4020-A5A2-C34F1B365E5B}" name="True Positives" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{7A2BA5DC-5762-4069-ABAF-1548014E1D14}" name="True Negatives" dataDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{22FBECAE-4DDE-4AFA-9C3F-DB9E683A9A2B}" name="False Positives" dataDxfId="29"/>
-    <tableColumn id="7" xr3:uid="{CB14F0E6-2F97-4C94-907D-5B473F04B319}" name="False Negatives" dataDxfId="28"/>
-    <tableColumn id="8" xr3:uid="{2B947D44-3F7F-46B9-887B-B617634ADD7E}" name="Threshold" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{D8E42556-2752-4020-A5A2-C34F1B365E5B}" name="True Positives" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{7A2BA5DC-5762-4069-ABAF-1548014E1D14}" name="True Negatives" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{22FBECAE-4DDE-4AFA-9C3F-DB9E683A9A2B}" name="False Positives" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{CB14F0E6-2F97-4C94-907D-5B473F04B319}" name="False Negatives" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{2B947D44-3F7F-46B9-887B-B617634ADD7E}" name="Threshold" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{70BD5F80-DC43-4179-B4CA-F459FC673450}" name="Table5" displayName="Table5" ref="B29:F32" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{70BD5F80-DC43-4179-B4CA-F459FC673450}" name="Table5" displayName="Table5" ref="B29:F32" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="B29:F32" xr:uid="{2E41160F-3EAF-48EF-A1E5-3A508AB6C2B6}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{89CDDEF4-2006-4CC2-8702-01D97ECD9FFE}" name="Aggregation mechanism" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{6F94AF4C-FE23-48EC-9CA2-82AD7DA29C2D}" name="k" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{1933BB4F-EFD7-44A6-A26C-AA85293D75AB}" name="cross-validation error" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{BE494206-5029-4AF8-8FF9-0751AB91C87B}" name="n" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{348B0B88-6665-4983-BAB7-C91E9E335308}" name="generalization error" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{89CDDEF4-2006-4CC2-8702-01D97ECD9FFE}" name="Aggregation mechanism" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{6F94AF4C-FE23-48EC-9CA2-82AD7DA29C2D}" name="k" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{1933BB4F-EFD7-44A6-A26C-AA85293D75AB}" name="cross-validation error" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{BE494206-5029-4AF8-8FF9-0751AB91C87B}" name="n" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{348B0B88-6665-4983-BAB7-C91E9E335308}" name="generalization error" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{25483E7F-88A1-4D45-A3DB-8811E9379E40}" name="Table13" displayName="Table13" ref="B3:F9" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{25483E7F-88A1-4D45-A3DB-8811E9379E40}" name="Table13" displayName="Table13" ref="B3:F9" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="B3:F9" xr:uid="{4EE24B2E-1496-4E1A-AD27-C2647F430286}"/>
   <sortState ref="B4:F9">
     <sortCondition ref="E3:E9"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="6" xr3:uid="{74D2DE9A-B30C-484D-BE41-296992A34AA9}" name="number of folds (k)" dataDxfId="17"/>
-    <tableColumn id="1" xr3:uid="{601B47CC-1D66-4216-BF9B-E9E4FF81F454}" name="Samples and sizes" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{3B6C7B2A-86F8-4582-9227-83370F3B25F7}" name="ROC AUC (Receiver Operator Curve Area Under the Curve)" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{D4A7C258-516A-4C68-B14F-A507710EFE7B}" name="Sensitivity Rate of True Positives" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{2FF3F640-5070-4972-B3F6-0ACEF875EE92}" name="Sensibility Rate of True Negatives" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{74D2DE9A-B30C-484D-BE41-296992A34AA9}" name="number of folds (k)" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{601B47CC-1D66-4216-BF9B-E9E4FF81F454}" name="Samples and sizes" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{3B6C7B2A-86F8-4582-9227-83370F3B25F7}" name="ROC AUC (Receiver Operator Curve Area Under the Curve)" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{D4A7C258-516A-4C68-B14F-A507710EFE7B}" name="Sensitivity Rate of True Positives" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{2FF3F640-5070-4972-B3F6-0ACEF875EE92}" name="Sensibility Rate of True Negatives" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -14867,30 +14961,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ECC3DC8-F219-4A35-9322-7470EB6D3D5C}">
   <dimension ref="B2:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="H21:I21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="19.54296875" customWidth="1"/>
-    <col min="3" max="3" width="13.54296875" customWidth="1"/>
+    <col min="2" max="2" width="19.53125" customWidth="1"/>
+    <col min="3" max="3" width="13.53125" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="10.36328125" customWidth="1"/>
-    <col min="7" max="7" width="10.453125" customWidth="1"/>
-    <col min="8" max="8" width="11.90625" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" customWidth="1"/>
+    <col min="7" max="7" width="10.46484375" customWidth="1"/>
+    <col min="8" max="8" width="11.9296875" customWidth="1"/>
     <col min="9" max="9" width="10" customWidth="1"/>
-    <col min="10" max="10" width="10.36328125" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" customWidth="1"/>
     <col min="12" max="12" width="11" customWidth="1"/>
-    <col min="13" max="13" width="11.1796875" customWidth="1"/>
+    <col min="13" max="13" width="11.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="2:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:13" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B3" s="16" t="s">
         <v>57</v>
       </c>
@@ -14928,7 +15022,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B4" s="19" t="s">
         <v>52</v>
       </c>
@@ -14966,7 +15060,7 @@
         <v>0.96153846153846201</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B5" s="19" t="s">
         <v>33</v>
       </c>
@@ -15004,7 +15098,7 @@
         <v>0.95192307692307698</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B6" s="19" t="s">
         <v>48</v>
       </c>
@@ -15042,7 +15136,7 @@
         <v>0.94230769230769196</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B7" s="19" t="s">
         <v>49</v>
       </c>
@@ -15080,7 +15174,7 @@
         <v>0.94230769230769196</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B8" s="19" t="s">
         <v>50</v>
       </c>
@@ -15118,7 +15212,7 @@
         <v>0.94230769230769196</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B9" s="19" t="s">
         <v>51</v>
       </c>
@@ -15156,7 +15250,7 @@
         <v>0.94230769230769196</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B10" s="19" t="s">
         <v>58</v>
       </c>
@@ -15194,7 +15288,7 @@
         <v>0.94230769230769196</v>
       </c>
     </row>
-    <row r="11" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B11" s="23" t="s">
         <v>59</v>
       </c>
@@ -15232,37 +15326,37 @@
         <v>0.86538461538461497</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B16" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B17" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
         <v>64</v>
       </c>
@@ -15277,6 +15371,117 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A399803E-BD6C-45A7-ABB7-1D5CC59B1772}">
+  <dimension ref="B3:B29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B16" s="27" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B23" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B24" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B27" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E905E9D4-D440-4A8A-92B2-D022498CC8E2}">
   <dimension ref="B1:H32"/>
   <sheetViews>
@@ -15284,21 +15489,21 @@
       <selection activeCell="D37" sqref="D37:D38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="17.9296875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="3.36328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="23.54296875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.90625" style="1"/>
-    <col min="4" max="4" width="20.7265625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="17.90625" style="1"/>
+    <col min="1" max="1" width="3.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.53125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.9296875" style="1"/>
+    <col min="4" max="4" width="20.73046875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="17.9296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B1" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B2" s="7" t="s">
         <v>29</v>
       </c>
@@ -15310,7 +15515,7 @@
         <v>6.2015503875968991E-2</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -15333,7 +15538,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="23" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:8" ht="23" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="1">
         <v>3</v>
       </c>
@@ -15357,7 +15562,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B5" s="1">
         <v>5</v>
       </c>
@@ -15381,7 +15586,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B6" s="1">
         <v>7</v>
       </c>
@@ -15405,7 +15610,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B7" s="1">
         <v>9</v>
       </c>
@@ -15429,7 +15634,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B8" s="1">
         <v>4</v>
       </c>
@@ -15453,7 +15658,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B9" s="1">
         <v>2</v>
       </c>
@@ -15477,7 +15682,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B10" s="1">
         <v>1</v>
       </c>
@@ -15501,15 +15706,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B12" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B13" s="3" t="s">
         <v>21</v>
       </c>
@@ -15518,7 +15723,7 @@
         <v>2.3255813953488413E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B14" s="2" t="s">
         <v>2</v>
       </c>
@@ -15541,7 +15746,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B15" s="1">
         <v>3</v>
       </c>
@@ -15565,7 +15770,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B16" s="1">
         <v>5</v>
       </c>
@@ -15589,7 +15794,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B17" s="1">
         <v>7</v>
       </c>
@@ -15613,7 +15818,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B18" s="1">
         <v>9</v>
       </c>
@@ -15637,12 +15842,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B20" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B21" s="3" t="s">
         <v>21</v>
       </c>
@@ -15651,7 +15856,7 @@
         <v>0.12403100775193798</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B22" s="2" t="s">
         <v>2</v>
       </c>
@@ -15674,7 +15879,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B23" s="1">
         <v>3</v>
       </c>
@@ -15698,7 +15903,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B24" s="1">
         <v>5</v>
       </c>
@@ -15722,7 +15927,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B25" s="1">
         <v>7</v>
       </c>
@@ -15746,7 +15951,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B26" s="1">
         <v>9</v>
       </c>
@@ -15770,7 +15975,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B29" s="2" t="s">
         <v>24</v>
       </c>
@@ -15787,7 +15992,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B30" s="4" t="s">
         <v>26</v>
       </c>
@@ -15803,7 +16008,7 @@
       </c>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B31" s="4" t="s">
         <v>27</v>
       </c>
@@ -15819,7 +16024,7 @@
       </c>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B32" s="4" t="s">
         <v>28</v>
       </c>
@@ -15847,7 +16052,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{103C3932-7911-4558-8622-359D7BC2E5F7}">
   <dimension ref="B2:F13"/>
   <sheetViews>
@@ -15855,22 +16060,22 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="17.9296875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="3.36328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.90625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.08984375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.54296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.9296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.06640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.53125" style="1" customWidth="1"/>
     <col min="5" max="5" width="21" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="17.90625" style="1"/>
+    <col min="6" max="16384" width="17.9296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -15887,7 +16092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="23" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" ht="23" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="4">
         <v>6</v>
       </c>
@@ -15904,7 +16109,7 @@
         <v>0.66666669999999995</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B5" s="4">
         <v>7</v>
       </c>
@@ -15921,7 +16126,7 @@
         <v>0.40476190000000001</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B6" s="4">
         <v>4</v>
       </c>
@@ -15938,7 +16143,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B7" s="4">
         <v>3</v>
       </c>
@@ -15955,7 +16160,7 @@
         <v>0.78333330000000001</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B8" s="4">
         <v>5</v>
       </c>
@@ -15972,7 +16177,7 @@
         <v>0.69333330000000004</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B9" s="4">
         <v>2</v>
       </c>
@@ -15989,10 +16194,10 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B13" s="3"/>
     </row>
   </sheetData>
@@ -16004,7 +16209,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25AEB740-6AE2-4FAF-80AD-192013CED4F1}">
   <dimension ref="B3:F23"/>
   <sheetViews>
@@ -16012,12 +16217,12 @@
       <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="5" max="5" width="10.36328125" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B3" s="11" t="s">
         <v>33</v>
       </c>
@@ -16034,7 +16239,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B4" s="11">
         <v>9</v>
       </c>
@@ -16051,7 +16256,7 @@
         <v>0.57638889999999998</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B5" s="11">
         <v>7</v>
       </c>
@@ -16068,7 +16273,7 @@
         <v>0.44675930000000003</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B6" s="11">
         <v>9</v>
       </c>
@@ -16085,7 +16290,7 @@
         <v>0.29970760000000002</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B7" s="11">
         <v>9</v>
       </c>
@@ -16102,7 +16307,7 @@
         <v>0.26941179999999998</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B8" s="11">
         <v>9</v>
       </c>
@@ -16119,7 +16324,7 @@
         <v>0.1140351</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B9" s="11">
         <v>9</v>
       </c>
@@ -16136,7 +16341,7 @@
         <v>0.1111111</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B10" s="11">
         <v>9</v>
       </c>
@@ -16153,7 +16358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B11" s="11">
         <v>9</v>
       </c>
@@ -16170,7 +16375,7 @@
         <v>6.6666669999999997E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B12" s="11">
         <v>7</v>
       </c>
@@ -16187,7 +16392,7 @@
         <v>6.1904760000000003E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B13" s="11">
         <v>5</v>
       </c>
@@ -16204,7 +16409,7 @@
         <v>0.15210546999999999</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B14" s="11">
         <v>7</v>
       </c>
@@ -16221,7 +16426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B15" s="11">
         <v>5</v>
       </c>
@@ -16238,7 +16443,7 @@
         <v>0.1433566</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B16" s="11">
         <v>5</v>
       </c>
@@ -16255,7 +16460,7 @@
         <v>0.19109461999999999</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B17" s="11">
         <v>5</v>
       </c>
@@ -16272,7 +16477,7 @@
         <v>0.15122654999999999</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.45">
       <c r="C19" t="s">
         <v>36</v>
       </c>
@@ -16280,7 +16485,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.45">
       <c r="C20" t="s">
         <v>37</v>
       </c>
@@ -16288,7 +16493,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.45">
       <c r="C22" t="s">
         <v>36</v>
       </c>
@@ -16296,273 +16501,11 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.45">
       <c r="C23" t="s">
         <v>37</v>
       </c>
       <c r="D23" t="s">
-        <v>41</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2C8D7A9-E1B8-40BF-BA41-272A23CF726B}">
-  <dimension ref="B3:E26"/>
-  <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:C26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="4" max="4" width="10.36328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B3" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B4" s="11">
-        <v>2</v>
-      </c>
-      <c r="C4" s="13">
-        <v>0.74426559999999997</v>
-      </c>
-      <c r="D4" s="12">
-        <v>0.88420270000000001</v>
-      </c>
-      <c r="E4" s="12">
-        <v>0.39743590000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B5" s="11">
-        <v>3</v>
-      </c>
-      <c r="C5" s="13">
-        <v>0.74897760000000002</v>
-      </c>
-      <c r="D5" s="12">
-        <v>0.88501399999999997</v>
-      </c>
-      <c r="E5" s="12">
-        <v>0.36797390000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B6" s="11">
-        <v>4</v>
-      </c>
-      <c r="C6" s="13">
-        <v>0.79843169999999997</v>
-      </c>
-      <c r="D6" s="12">
-        <v>0.90111189999999997</v>
-      </c>
-      <c r="E6" s="12">
-        <v>0.50481149999999997</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B7" s="11">
-        <v>5</v>
-      </c>
-      <c r="C7" s="13">
-        <v>0.79373950000000004</v>
-      </c>
-      <c r="D7" s="12">
-        <v>0.89502559999999998</v>
-      </c>
-      <c r="E7" s="12">
-        <v>0.44262629999999997</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B8" s="11">
-        <v>6</v>
-      </c>
-      <c r="C8" s="13">
-        <v>0.78321600000000002</v>
-      </c>
-      <c r="D8" s="12">
-        <v>0.87937900000000002</v>
-      </c>
-      <c r="E8" s="12">
-        <v>0.45287840000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B9" s="11">
-        <v>7</v>
-      </c>
-      <c r="C9" s="13">
-        <v>0.74757709999999999</v>
-      </c>
-      <c r="D9" s="12">
-        <v>0.88080170000000002</v>
-      </c>
-      <c r="E9" s="12">
-        <v>0.48282829999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B10" s="11">
-        <v>8</v>
-      </c>
-      <c r="C10" s="13">
-        <v>0.78290780000000004</v>
-      </c>
-      <c r="D10" s="12">
-        <v>0.89143660000000002</v>
-      </c>
-      <c r="E10" s="12">
-        <v>0.52457589999999998</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B11" s="11">
-        <v>9</v>
-      </c>
-      <c r="C11" s="13">
-        <v>0.75931309999999996</v>
-      </c>
-      <c r="D11" s="12">
-        <v>0.85155139999999996</v>
-      </c>
-      <c r="E11" s="12">
-        <v>0.43992720000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B12" s="11">
-        <v>10</v>
-      </c>
-      <c r="C12" s="13">
-        <v>0.79550209999999999</v>
-      </c>
-      <c r="D12" s="12">
-        <v>0.88832580000000005</v>
-      </c>
-      <c r="E12" s="12">
-        <v>0.47679510000000003</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B13" s="11">
-        <v>11</v>
-      </c>
-      <c r="C13" s="13">
-        <v>0.78559120000000005</v>
-      </c>
-      <c r="D13" s="12">
-        <v>0.88347010000000004</v>
-      </c>
-      <c r="E13" s="12">
-        <v>0.48625580000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B14" s="11">
-        <v>12</v>
-      </c>
-      <c r="C14" s="13">
-        <v>0.79879560000000005</v>
-      </c>
-      <c r="D14" s="12">
-        <v>0.91136539999999999</v>
-      </c>
-      <c r="E14" s="12">
-        <v>0.42298570000000002</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B15" s="11">
-        <v>13</v>
-      </c>
-      <c r="C15" s="13">
-        <v>0.79263499999999998</v>
-      </c>
-      <c r="D15" s="12">
-        <v>0.88334979999999996</v>
-      </c>
-      <c r="E15" s="12">
-        <v>0.43476989999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B16" s="11">
-        <v>14</v>
-      </c>
-      <c r="C16" s="13">
-        <v>0.76653179999999999</v>
-      </c>
-      <c r="D16" s="12">
-        <v>0.86783449999999995</v>
-      </c>
-      <c r="E16" s="12">
-        <v>0.44531009999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B17" s="11">
-        <v>15</v>
-      </c>
-      <c r="C17" s="13">
-        <v>0.76647030000000005</v>
-      </c>
-      <c r="D17" s="12">
-        <v>0.83289279999999999</v>
-      </c>
-      <c r="E17" s="12">
-        <v>0.52724230000000005</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B23" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B25" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B26" t="s">
-        <v>37</v>
-      </c>
-      <c r="C26" t="s">
         <v>41</v>
       </c>
     </row>
@@ -16574,19 +16517,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19383C2D-EDF0-42FD-AA00-4CF79188BCEB}">
-  <dimension ref="B3:E23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2C8D7A9-E1B8-40BF-BA41-272A23CF726B}">
+  <dimension ref="B3:E26"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:C23"/>
+    <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="4" max="4" width="10.36328125" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B3" s="11" t="s">
         <v>34</v>
       </c>
@@ -16600,231 +16543,231 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B4" s="11">
         <v>2</v>
       </c>
-      <c r="C4" s="10">
-        <v>0.9426563</v>
+      <c r="C4" s="13">
+        <v>0.74426559999999997</v>
       </c>
       <c r="D4" s="12">
-        <v>0.87938079999999996</v>
+        <v>0.88420270000000001</v>
       </c>
       <c r="E4" s="12">
-        <v>0.51923079999999999</v>
+        <v>0.39743590000000001</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B5" s="11">
         <v>3</v>
       </c>
-      <c r="C5" s="10">
-        <v>0.87959220000000005</v>
+      <c r="C5" s="13">
+        <v>0.74897760000000002</v>
       </c>
       <c r="D5" s="12">
-        <v>0.93761209999999995</v>
+        <v>0.88501399999999997</v>
       </c>
       <c r="E5" s="12">
-        <v>0.45955879999999999</v>
+        <v>0.36797390000000002</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B6" s="11">
         <v>4</v>
       </c>
-      <c r="C6" s="10">
-        <v>0.87870119999999996</v>
+      <c r="C6" s="13">
+        <v>0.79843169999999997</v>
       </c>
       <c r="D6" s="12">
-        <v>0.94546699999999995</v>
+        <v>0.90111189999999997</v>
       </c>
       <c r="E6" s="12">
-        <v>0.48369879999999998</v>
+        <v>0.50481149999999997</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B7" s="11">
         <v>5</v>
       </c>
-      <c r="C7" s="10">
-        <v>0.87955559999999999</v>
+      <c r="C7" s="13">
+        <v>0.79373950000000004</v>
       </c>
       <c r="D7" s="12">
-        <v>0.94278039999999996</v>
+        <v>0.89502559999999998</v>
       </c>
       <c r="E7" s="12">
-        <v>0.51846890000000001</v>
+        <v>0.44262629999999997</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B8" s="11">
         <v>6</v>
       </c>
-      <c r="C8" s="10">
-        <v>0.88117140000000005</v>
+      <c r="C8" s="13">
+        <v>0.78321600000000002</v>
       </c>
       <c r="D8" s="12">
-        <v>0.92817450000000001</v>
+        <v>0.87937900000000002</v>
       </c>
       <c r="E8" s="12">
-        <v>0.4854427</v>
+        <v>0.45287840000000001</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B9" s="11">
         <v>7</v>
       </c>
-      <c r="C9" s="10">
-        <v>0.87983339999999999</v>
+      <c r="C9" s="13">
+        <v>0.74757709999999999</v>
       </c>
       <c r="D9" s="12">
-        <v>0.94267970000000001</v>
+        <v>0.88080170000000002</v>
       </c>
       <c r="E9" s="12">
-        <v>0.45571080000000003</v>
+        <v>0.48282829999999999</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B10" s="11">
         <v>8</v>
       </c>
-      <c r="C10" s="10">
-        <v>0.87945989999999996</v>
+      <c r="C10" s="13">
+        <v>0.78290780000000004</v>
       </c>
       <c r="D10" s="12">
-        <v>0.93582390000000004</v>
+        <v>0.89143660000000002</v>
       </c>
       <c r="E10" s="12">
-        <v>0.45945619999999998</v>
+        <v>0.52457589999999998</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B11" s="11">
         <v>9</v>
       </c>
-      <c r="C11" s="10">
-        <v>0.87965579999999999</v>
+      <c r="C11" s="13">
+        <v>0.75931309999999996</v>
       </c>
       <c r="D11" s="12">
-        <v>0.93382869999999996</v>
+        <v>0.85155139999999996</v>
       </c>
       <c r="E11" s="12">
-        <v>0.4622985</v>
+        <v>0.43992720000000002</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B12" s="11">
         <v>10</v>
       </c>
-      <c r="C12" s="10">
-        <v>0.87925469999999994</v>
+      <c r="C12" s="13">
+        <v>0.79550209999999999</v>
       </c>
       <c r="D12" s="12">
-        <v>0.93309830000000005</v>
+        <v>0.88832580000000005</v>
       </c>
       <c r="E12" s="12">
-        <v>0.41729719999999998</v>
+        <v>0.47679510000000003</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B13" s="11">
         <v>11</v>
       </c>
-      <c r="C13" s="10">
-        <v>0.87910889999999997</v>
+      <c r="C13" s="13">
+        <v>0.78559120000000005</v>
       </c>
       <c r="D13" s="12">
-        <v>0.93691630000000004</v>
+        <v>0.88347010000000004</v>
       </c>
       <c r="E13" s="12">
-        <v>0.44673439999999998</v>
+        <v>0.48625580000000002</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B14" s="11">
         <v>12</v>
       </c>
-      <c r="C14" s="10">
-        <v>0.87934000000000001</v>
+      <c r="C14" s="13">
+        <v>0.79879560000000005</v>
       </c>
       <c r="D14" s="12">
-        <v>0.94082200000000005</v>
+        <v>0.91136539999999999</v>
       </c>
       <c r="E14" s="12">
-        <v>0.46603260000000002</v>
+        <v>0.42298570000000002</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B15" s="11">
         <v>13</v>
       </c>
-      <c r="C15" s="10">
-        <v>0.87934009999999996</v>
+      <c r="C15" s="13">
+        <v>0.79263499999999998</v>
       </c>
       <c r="D15" s="12">
-        <v>0.92233050000000005</v>
+        <v>0.88334979999999996</v>
       </c>
       <c r="E15" s="12">
-        <v>0.46362330000000002</v>
+        <v>0.43476989999999999</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B16" s="11">
         <v>14</v>
       </c>
-      <c r="C16" s="10">
-        <v>0.85163390000000005</v>
+      <c r="C16" s="13">
+        <v>0.76653179999999999</v>
       </c>
       <c r="D16" s="12">
-        <v>0.91542869999999998</v>
+        <v>0.86783449999999995</v>
       </c>
       <c r="E16" s="12">
-        <v>0.45166339999999999</v>
+        <v>0.44531009999999999</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B17" s="11">
         <v>15</v>
       </c>
-      <c r="C17" s="10">
-        <v>0.82778890000000005</v>
+      <c r="C17" s="13">
+        <v>0.76647030000000005</v>
       </c>
       <c r="D17" s="12">
-        <v>0.91993599999999998</v>
+        <v>0.83289279999999999</v>
       </c>
       <c r="E17" s="12">
-        <v>0.48937199999999997</v>
+        <v>0.52724230000000005</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B20" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
         <v>36</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B23" t="s">
         <v>37</v>
       </c>
       <c r="C23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" t="s">
         <v>41</v>
       </c>
     </row>
@@ -16836,6 +16779,268 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19383C2D-EDF0-42FD-AA00-4CF79188BCEB}">
+  <dimension ref="B3:E23"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B3" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B4" s="11">
+        <v>2</v>
+      </c>
+      <c r="C4" s="10">
+        <v>0.9426563</v>
+      </c>
+      <c r="D4" s="12">
+        <v>0.87938079999999996</v>
+      </c>
+      <c r="E4" s="12">
+        <v>0.51923079999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B5" s="11">
+        <v>3</v>
+      </c>
+      <c r="C5" s="10">
+        <v>0.87959220000000005</v>
+      </c>
+      <c r="D5" s="12">
+        <v>0.93761209999999995</v>
+      </c>
+      <c r="E5" s="12">
+        <v>0.45955879999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B6" s="11">
+        <v>4</v>
+      </c>
+      <c r="C6" s="10">
+        <v>0.87870119999999996</v>
+      </c>
+      <c r="D6" s="12">
+        <v>0.94546699999999995</v>
+      </c>
+      <c r="E6" s="12">
+        <v>0.48369879999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B7" s="11">
+        <v>5</v>
+      </c>
+      <c r="C7" s="10">
+        <v>0.87955559999999999</v>
+      </c>
+      <c r="D7" s="12">
+        <v>0.94278039999999996</v>
+      </c>
+      <c r="E7" s="12">
+        <v>0.51846890000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B8" s="11">
+        <v>6</v>
+      </c>
+      <c r="C8" s="10">
+        <v>0.88117140000000005</v>
+      </c>
+      <c r="D8" s="12">
+        <v>0.92817450000000001</v>
+      </c>
+      <c r="E8" s="12">
+        <v>0.4854427</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B9" s="11">
+        <v>7</v>
+      </c>
+      <c r="C9" s="10">
+        <v>0.87983339999999999</v>
+      </c>
+      <c r="D9" s="12">
+        <v>0.94267970000000001</v>
+      </c>
+      <c r="E9" s="12">
+        <v>0.45571080000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B10" s="11">
+        <v>8</v>
+      </c>
+      <c r="C10" s="10">
+        <v>0.87945989999999996</v>
+      </c>
+      <c r="D10" s="12">
+        <v>0.93582390000000004</v>
+      </c>
+      <c r="E10" s="12">
+        <v>0.45945619999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B11" s="11">
+        <v>9</v>
+      </c>
+      <c r="C11" s="10">
+        <v>0.87965579999999999</v>
+      </c>
+      <c r="D11" s="12">
+        <v>0.93382869999999996</v>
+      </c>
+      <c r="E11" s="12">
+        <v>0.4622985</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B12" s="11">
+        <v>10</v>
+      </c>
+      <c r="C12" s="10">
+        <v>0.87925469999999994</v>
+      </c>
+      <c r="D12" s="12">
+        <v>0.93309830000000005</v>
+      </c>
+      <c r="E12" s="12">
+        <v>0.41729719999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B13" s="11">
+        <v>11</v>
+      </c>
+      <c r="C13" s="10">
+        <v>0.87910889999999997</v>
+      </c>
+      <c r="D13" s="12">
+        <v>0.93691630000000004</v>
+      </c>
+      <c r="E13" s="12">
+        <v>0.44673439999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B14" s="11">
+        <v>12</v>
+      </c>
+      <c r="C14" s="10">
+        <v>0.87934000000000001</v>
+      </c>
+      <c r="D14" s="12">
+        <v>0.94082200000000005</v>
+      </c>
+      <c r="E14" s="12">
+        <v>0.46603260000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B15" s="11">
+        <v>13</v>
+      </c>
+      <c r="C15" s="10">
+        <v>0.87934009999999996</v>
+      </c>
+      <c r="D15" s="12">
+        <v>0.92233050000000005</v>
+      </c>
+      <c r="E15" s="12">
+        <v>0.46362330000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B16" s="11">
+        <v>14</v>
+      </c>
+      <c r="C16" s="10">
+        <v>0.85163390000000005</v>
+      </c>
+      <c r="D16" s="12">
+        <v>0.91542869999999998</v>
+      </c>
+      <c r="E16" s="12">
+        <v>0.45166339999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B17" s="11">
+        <v>15</v>
+      </c>
+      <c r="C17" s="10">
+        <v>0.82778890000000005</v>
+      </c>
+      <c r="D17" s="12">
+        <v>0.91993599999999998</v>
+      </c>
+      <c r="E17" s="12">
+        <v>0.48937199999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5CE95F2-2905-4F40-965A-C017CDB146E7}">
   <dimension ref="B3:O32"/>
   <sheetViews>
@@ -16843,13 +17048,13 @@
       <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" customWidth="1"/>
-    <col min="4" max="4" width="10.36328125" customWidth="1"/>
+    <col min="1" max="1" width="8.73046875" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B3" s="11" t="s">
         <v>34</v>
       </c>
@@ -16863,7 +17068,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B4" s="11">
         <v>2</v>
       </c>
@@ -16877,7 +17082,7 @@
         <v>0.3333333</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B5" s="11">
         <v>3</v>
       </c>
@@ -16891,7 +17096,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B6" s="11">
         <v>4</v>
       </c>
@@ -16905,7 +17110,7 @@
         <v>0.20789469999999999</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B7" s="11">
         <v>5</v>
       </c>
@@ -16919,7 +17124,7 @@
         <v>0.72245610000000005</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B8" s="11">
         <v>6</v>
       </c>
@@ -16933,7 +17138,7 @@
         <v>0.42902709999999999</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B9" s="11">
         <v>7</v>
       </c>
@@ -16947,7 +17152,7 @@
         <v>0.53821892000000005</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B10" s="11">
         <v>8</v>
       </c>
@@ -16961,7 +17166,7 @@
         <v>0.25085809999999997</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B11" s="11">
         <v>9</v>
       </c>
@@ -16975,7 +17180,7 @@
         <v>0.54287178000000003</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B12" s="11">
         <v>10</v>
       </c>
@@ -16989,7 +17194,7 @@
         <v>0.24783549999999999</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B13" s="11">
         <v>11</v>
       </c>
@@ -17003,7 +17208,7 @@
         <v>0.34288540000000001</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B14" s="11">
         <v>12</v>
       </c>
@@ -17017,7 +17222,7 @@
         <v>0.29262700000000003</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B15" s="11">
         <v>13</v>
       </c>
@@ -17031,7 +17236,7 @@
         <v>0.20521793999999999</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B16" s="11">
         <v>14</v>
       </c>
@@ -17045,7 +17250,7 @@
         <v>0.37009730000000002</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.45">
       <c r="B17" s="11">
         <v>15</v>
       </c>
@@ -17059,7 +17264,7 @@
         <v>0.63246990000000003</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.45">
       <c r="B18" s="11">
         <v>30</v>
       </c>
@@ -17073,7 +17278,7 @@
         <v>0.72826089999999999</v>
       </c>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.45">
       <c r="B19" s="11">
         <v>45</v>
       </c>
@@ -17087,7 +17292,7 @@
         <v>0.497807</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.45">
       <c r="B20" s="11">
         <v>60</v>
       </c>
@@ -17104,7 +17309,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.45">
       <c r="B21" s="11">
         <v>70</v>
       </c>
@@ -17118,7 +17323,7 @@
         <v>0.69246030000000003</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.45">
       <c r="B22" s="11">
         <v>75</v>
       </c>
@@ -17132,7 +17337,7 @@
         <v>0.61979169999999995</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.45">
       <c r="B23" s="11">
         <v>90</v>
       </c>
@@ -17146,7 +17351,7 @@
         <v>0.76515149999999998</v>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.45">
       <c r="B24" s="11">
         <v>100</v>
       </c>
@@ -17160,7 +17365,7 @@
         <v>0.80952380000000002</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.45">
       <c r="B25" s="11">
         <v>115</v>
       </c>
@@ -17174,7 +17379,7 @@
         <v>0.83333330000000005</v>
       </c>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.45">
       <c r="B27" t="s">
         <v>35</v>
       </c>
@@ -17182,7 +17387,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
         <v>36</v>
       </c>
@@ -17190,7 +17395,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.45">
       <c r="B29" t="s">
         <v>37</v>
       </c>
@@ -17198,7 +17403,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.45">
       <c r="B31" t="s">
         <v>36</v>
       </c>
@@ -17206,7 +17411,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:15" x14ac:dyDescent="0.45">
       <c r="B32" t="s">
         <v>37</v>
       </c>

</xml_diff>